<commit_message>
Have all potential data sources entered and noted
</commit_message>
<xml_diff>
--- a/DADA-Forest.xlsx
+++ b/DADA-Forest.xlsx
@@ -5,11 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData Sources" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="National Forest Service" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Office of the Chief" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Business Operations" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="National Forest Service" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Forest Service Research and Dev" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="State, Private, and Tribal Fore" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Notes and Comments" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="120">
   <si>
     <t xml:space="preserve">Ref. Resources:</t>
   </si>
@@ -356,44 +361,26 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes: Many sites have links to items like pdf documents and spreadsheets.  These items seem like valuable data sources, but there is no metadata associated with them.
+    <t xml:space="preserve">Page does not seem to have any data or links to data sources that might be metadata sources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Page does not seem to have any data or links to data sources that might be metadata sources.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Possible, but not likely metadata sources at interface that allows for wildflower viewing queries.</t>
   </si>
   <si>
     <t xml:space="preserve">Possible metadata source at site’s geospatial link, but that link is dead.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Possible source via mapviewer link, 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Second possible source via the Regional Appraisal Data link 
+    <t xml:space="preserve">Possible source via mapviewer link, 
+Second possible source via the Regional Appraisal Data link 
 RAVG:https://www.fs.usda.gov/forestmanagement/products/appraisal-data.shtml)
 https://burnseverity.cr.usgs.gov/ravg/data-access
 Forest Vegetation Simulator?
 Forest Products Measurement?
 Forest Operations Equipment Catalog</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">https://data.fs.usda.gov/geodata/maps/standard-map.php
@@ -414,6 +401,9 @@
   <si>
     <t xml:space="preserve">TEUI?</t>
   </si>
+  <si>
+    <t xml:space="preserve">Notes: Many sites have links to items like pdf documents and spreadsheets.  These items seem like valuable data sources, but there is no metadata associated with them.</t>
+  </si>
 </sst>
 </file>
 
@@ -422,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,12 +476,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -550,7 +534,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,28 +567,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -612,14 +584,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -875,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="C7 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1429,12 +1409,14 @@
     <hyperlink ref="C1" r:id="rId1" display="https://www.fs.usda.gov/about-agency/national-programs-offices"/>
     <hyperlink ref="C2" r:id="rId2" display="https://www.fs.usda.gov/about-agency/organization"/>
     <hyperlink ref="A5" r:id="rId3" display="This matrix is based on programs described on the USFS Organization website."/>
+    <hyperlink ref="A8" location="Office of the Chief!A1" display="Office of the Chief"/>
     <hyperlink ref="C9" r:id="rId4" display="https://www.fs.usda.gov/about-agency/newsroom/leadership-biographies"/>
     <hyperlink ref="C10" r:id="rId5" display="https://www.fs.usda.gov/about-agency/civil-rights"/>
     <hyperlink ref="C11" r:id="rId6" display="https://www.fs.usda.gov/about-agency/international-programs/contact-us"/>
     <hyperlink ref="C12" r:id="rId7" display="https://www.fs.usda.gov/about-agency/contact-us/lei"/>
     <hyperlink ref="C13" r:id="rId8" display="https://www.fs.usda.gov/about-agency/contact-us/legislative-affairs"/>
     <hyperlink ref="C14" r:id="rId9" display="https://www.fs.usda.gov/about-agency/contact-us/office-communication"/>
+    <hyperlink ref="A16" location="Business Operations!A1" display="Business Operations"/>
     <hyperlink ref="C18" r:id="rId10" display="https://www.fs.usda.gov/working-with-us/grants"/>
     <hyperlink ref="C19" r:id="rId11" display="https://www.fs.usda.gov/business/"/>
     <hyperlink ref="C20" r:id="rId12" display="https://www.fs.usda.gov/about-agency/cio"/>
@@ -1445,7 +1427,7 @@
     <hyperlink ref="C28" r:id="rId17" display="https://www.fs.usda.gov/safety/contacts.shtml"/>
     <hyperlink ref="C29" r:id="rId18" display="https://www.fs.usda.gov/orms/"/>
     <hyperlink ref="C30" r:id="rId19" display="https://www.fs.usda.gov/strategicplan"/>
-    <hyperlink ref="A32" location="National Forest Service!A1" display="National Forest System"/>
+    <hyperlink ref="A32" location="'National Forest Service'!A1" display="National Forest System"/>
     <hyperlink ref="C33" r:id="rId20" display="https://www.fs.usda.gov/naturalresources/index.shtml"/>
     <hyperlink ref="C34" r:id="rId21" display="https://www.fs.usda.gov/managing-land/wildflowers"/>
     <hyperlink ref="C35" r:id="rId22" display="https://www.fs.usda.gov/about-agency/emc"/>
@@ -1467,7 +1449,9 @@
     <hyperlink ref="C52" r:id="rId38" display="https://www.fs.usda.gov/soils/index.shtml"/>
     <hyperlink ref="C53" r:id="rId39" display="https://www.fs.usda.gov/wild-horse-burro/index.shtml"/>
     <hyperlink ref="C54" r:id="rId40" display="https://www.fs.usda.gov/managing-land/wild-scenic-rivers"/>
+    <hyperlink ref="A56" location="Forest Service Research and Development" display="Forest Service Research and Development"/>
     <hyperlink ref="C57" r:id="rId41" display="https://www.fs.usda.gov/research/"/>
+    <hyperlink ref="A59" location="State, Private, and Tribal Forestry" display="State, Private, and Tribal Forestry"/>
     <hyperlink ref="C60" r:id="rId42" display="https://www.fs.usda.gov/about-agency/state-private-forestry"/>
     <hyperlink ref="C61" r:id="rId43" display="https://www.fs.usda.gov/main/conservationeducation/home"/>
     <hyperlink ref="C62" r:id="rId44" display="https://www.fs.usda.gov/about-agency/state-private-forestry/coop-forestry"/>
@@ -1492,358 +1476,642 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="57.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="90.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="100.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="13.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="32.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="9" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="48.93"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.fs.usda.gov/about-agency/newsroom/leadership-biographies"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.fs.usda.gov/about-agency/civil-rights"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.fs.usda.gov/about-agency/international-programs/contact-us"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.fs.usda.gov/about-agency/contact-us/lei"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.fs.usda.gov/about-agency/contact-us/legislative-affairs"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.fs.usda.gov/about-agency/contact-us/office-communication"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="C7 C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="54.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="74.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="43.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.fs.usda.gov/working-with-us/grants"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.fs.usda.gov/business/"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.fs.usda.gov/about-agency/cio"/>
+    <hyperlink ref="B8" r:id="rId4" display="https://www.fs.usda.gov/about-agency/foia"/>
+    <hyperlink ref="B9" r:id="rId5" display="https://www.fs.usda.gov/enterprise/"/>
+    <hyperlink ref="B10" r:id="rId6" display="https://www.fs.usda.gov/about-agency/contact-us/human-resources"/>
+    <hyperlink ref="B11" r:id="rId7" display="https://www.fs.usda.gov/working-with-us/careers/job-corps"/>
+    <hyperlink ref="B13" r:id="rId8" display="https://www.fs.usda.gov/safety/contacts.shtml"/>
+    <hyperlink ref="B14" r:id="rId9" display="https://www.fs.usda.gov/orms/"/>
+    <hyperlink ref="B15" r:id="rId10" display="https://www.fs.usda.gov/strategicplan"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C7 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="57.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="100.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="1" width="13.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>112</v>
+      <c r="C8" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>112</v>
+      <c r="C9" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>112</v>
+      <c r="C10" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>112</v>
+      <c r="C12" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>112</v>
+      <c r="C13" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>112</v>
+      <c r="C14" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>112</v>
+      <c r="C15" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>112</v>
+      <c r="C17" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>77</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>112</v>
+      <c r="C18" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>112</v>
+      <c r="C19" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>112</v>
+      <c r="C20" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>112</v>
+      <c r="C22" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>112</v>
+      <c r="C23" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
       <c r="B24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:Q1"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://www.fs.usda.gov/naturalresources/index.shtml"/>
     <hyperlink ref="B3" r:id="rId2" display="https://www.fs.usda.gov/managing-land/wildflowers"/>
@@ -1876,4 +2144,225 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="C7 C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="36.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="38.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="49.73"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.fs.usda.gov/research/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="C7 C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="39.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="80.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="47.29"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.fs.usda.gov/about-agency/state-private-forestry"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.fs.usda.gov/main/conservationeducation/home"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.fs.usda.gov/about-agency/state-private-forestry/coop-forestry"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.fs.usda.gov/nsl/index.html"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.fs.usda.gov/managing-land/fire/aviation"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.fs.usda.gov/foresthealth/index.shtml"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.fs.usda.gov/spf/tribalrelations/"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.fs.usda.gov/managing-land/urban-forests/ucf"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C7 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>